<commit_message>
Further work on exploring my hypothesis -- making some progress on the coding, but yet to come up with any good visuals to begin providing some evidence to answer my question.
</commit_message>
<xml_diff>
--- a/Invertebrates in R/inverts_class_data.xlsx
+++ b/Invertebrates in R/inverts_class_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GBC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorharrington/Library/Mobile Documents/com~apple~CloudDocs/School/23SPDAY/BioInformatics/GITHub/BioStatisticalAnalysis/Invertebrates in R/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2CA493-DC74-E742-A682-EA00DE4FFB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Site</t>
   </si>
@@ -99,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Riffle </t>
-  </si>
-  <si>
-    <t>1(upstream)</t>
   </si>
   <si>
     <t>Pool</t>
@@ -113,7 +111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,28 +422,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="6" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" customWidth="1"/>
+    <col min="2" max="6" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -587,12 +585,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -658,9 +656,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -729,12 +727,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>0.18</v>

</xml_diff>